<commit_message>
Correcciones en Perfil de Empleados
</commit_message>
<xml_diff>
--- a/Documentos/Reportes de Pruebas/Pruebas ASN_PE.xlsx
+++ b/Documentos/Reportes de Pruebas/Pruebas ASN_PE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t xml:space="preserve">CASO</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t xml:space="preserve">Campo Programa selección uno o todos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No permite seleccionar tipo de contrato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No aparece perfil de empleado creado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editamos perfil ya creado pero no guarda cambio en el campo cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASO04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orden Alfabético en el listado de clientes </t>
   </si>
 </sst>
 </file>
@@ -57,11 +72,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -79,9 +95,16 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,7 +149,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -139,7 +162,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -160,62 +191,106 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="57.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>44006</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>44006</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>44006</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>44009</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>44009</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>44009</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>44009</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección a edición de Perfil de Empleados
</commit_message>
<xml_diff>
--- a/Documentos/Reportes de Pruebas/Pruebas ASN_PE.xlsx
+++ b/Documentos/Reportes de Pruebas/Pruebas ASN_PE.xlsx
@@ -8,7 +8,14 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Reporte de Pendientes Pruebas Payroll Requests" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="CASO01 24-06-2020" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CASO02 24-06-20" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="CASO03 24-06-20" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="CASO01 27-06-20" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="CASO02 27-06-20" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="CASO03 27-06-20" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="CASO04 27-06-20" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t xml:space="preserve">CASO</t>
   </si>
@@ -31,21 +38,27 @@
     <t xml:space="preserve">Descripción</t>
   </si>
   <si>
+    <t xml:space="preserve">Liberado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmar pruebas</t>
+  </si>
+  <si>
     <t xml:space="preserve">CASO01</t>
   </si>
   <si>
     <t xml:space="preserve">Crear nuevo perfil de empleado </t>
   </si>
   <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
     <t xml:space="preserve">CASO02</t>
   </si>
   <si>
     <t xml:space="preserve">Edición de un Perfil ya existente</t>
   </si>
   <si>
-    <t xml:space="preserve">OK</t>
-  </si>
-  <si>
     <t xml:space="preserve">CASO03</t>
   </si>
   <si>
@@ -65,6 +78,21 @@
   </si>
   <si>
     <t xml:space="preserve">Orden Alfabético en el listado de clientes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrección</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORRECCIÓN: Es correcto. Los únicos campos que permiten múltiples selecciones son Cliente y Concepto de Nómina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORRECCIÓN: Ya se permite seleccionar Tipo de Contrato y Concepto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORRECCION: Ya puede seleccionarse el Cliente reportado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORRECCIÓN: Ya aparecen los clientes ordenados alfabéticamente.</t>
   </si>
 </sst>
 </file>
@@ -147,7 +175,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,6 +200,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,15 +216,410 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>733680</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>20880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Imagen 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9674280" cy="5385240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>255960</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>42480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>109800</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Imagen 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="255960" y="6544800"/>
+          <a:ext cx="5543280" cy="5265360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>328320</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3579480" cy="3731400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>502200</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>14400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 6" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4226400"/>
+          <a:ext cx="5378760" cy="5378760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123480</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6625800" cy="3667680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7560</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>441000</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>120600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5697000" y="4226400"/>
+          <a:ext cx="5310360" cy="5322600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>748440</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>24480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="360" y="4219200"/>
+          <a:ext cx="5624640" cy="5396040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>80280</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="360" y="0"/>
+          <a:ext cx="6582240" cy="3646800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>117000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>111600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 9" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6619320" cy="3687840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>14400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>99000</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>34200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 10" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4240800"/>
+          <a:ext cx="6601320" cy="6684840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -200,7 +627,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="57.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -213,52 +642,61 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>44006</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>44006</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>44006</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>44009</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -266,24 +704,27 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>44009</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>44009</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -291,13 +732,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>44009</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -312,4 +753,225 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B55" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J60" activeCellId="0" sqref="J60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4"/>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J28" activeCellId="0" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>